<commit_message>
Matrix of Class_SRS , new version of SRS
</commit_message>
<xml_diff>
--- a/MatrixClass_SRS.xlsx
+++ b/MatrixClass_SRS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QI YE\Documents\GitHub\SW_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\542115511\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Class / SRS</t>
   </si>
@@ -99,6 +99,126 @@
   </si>
   <si>
     <t>Administrator</t>
+  </si>
+  <si>
+    <t>SRS01</t>
+  </si>
+  <si>
+    <t>SRS02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS03 </t>
+  </si>
+  <si>
+    <t>SRS04</t>
+  </si>
+  <si>
+    <t>SRS05</t>
+  </si>
+  <si>
+    <t>SRS06</t>
+  </si>
+  <si>
+    <t>SRS07</t>
+  </si>
+  <si>
+    <t>SRS08</t>
+  </si>
+  <si>
+    <t>SRS09</t>
+  </si>
+  <si>
+    <t>SRS10</t>
+  </si>
+  <si>
+    <t>SRS11</t>
+  </si>
+  <si>
+    <t>SRS12</t>
+  </si>
+  <si>
+    <t>SRS13</t>
+  </si>
+  <si>
+    <t>SRS14</t>
+  </si>
+  <si>
+    <t>SRS15</t>
+  </si>
+  <si>
+    <t>SRS16</t>
+  </si>
+  <si>
+    <t>SRS17</t>
+  </si>
+  <si>
+    <t>SRS18</t>
+  </si>
+  <si>
+    <t>SRS19</t>
+  </si>
+  <si>
+    <t>SRS20</t>
+  </si>
+  <si>
+    <t>SRS21</t>
+  </si>
+  <si>
+    <t>SRS22</t>
+  </si>
+  <si>
+    <t>SRS23</t>
+  </si>
+  <si>
+    <t>SRS24</t>
+  </si>
+  <si>
+    <t>SRS25</t>
+  </si>
+  <si>
+    <t>SRS26</t>
+  </si>
+  <si>
+    <t>SRS27</t>
+  </si>
+  <si>
+    <t>SRS28</t>
+  </si>
+  <si>
+    <t>SRS29</t>
+  </si>
+  <si>
+    <t>SRS30</t>
+  </si>
+  <si>
+    <t>SRS31</t>
+  </si>
+  <si>
+    <t>SRS32</t>
+  </si>
+  <si>
+    <t>SRS33</t>
+  </si>
+  <si>
+    <t>SRS34</t>
+  </si>
+  <si>
+    <t>SRS35</t>
+  </si>
+  <si>
+    <t>SRS36</t>
+  </si>
+  <si>
+    <t>SRS37</t>
+  </si>
+  <si>
+    <t>SRS38</t>
+  </si>
+  <si>
+    <t>SRS39</t>
+  </si>
+  <si>
+    <t>SRS40</t>
   </si>
 </sst>
 </file>
@@ -114,12 +234,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -134,8 +260,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:AO25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -427,130 +555,319 @@
     <col min="1" max="1" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V1" t="s">
+        <v>45</v>
+      </c>
+      <c r="W1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="S3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="M7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="AG7" s="1"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="Z9" s="1"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="Q10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AI11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AO11" s="1"/>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AK13" s="1"/>
+      <c r="AN13" s="1"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="W16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AD17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AN17" s="1"/>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AC20" s="1"/>
+      <c r="AE20" s="1"/>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="W21" s="1"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="1"/>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="1"/>
+      <c r="AN22" s="1"/>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AA23" s="1"/>
+      <c r="AD23" s="1"/>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AH24" s="1"/>
+      <c r="AN24" s="1"/>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
+      <c r="F25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="AI25" s="2"/>
+      <c r="AL25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>